<commit_message>
Final update with experiments
</commit_message>
<xml_diff>
--- a/extensions/icdm2016/doc-Experiments/GlobalHiddenVSUnemploymentRate.xlsx
+++ b/extensions/icdm2016/doc-Experiments/GlobalHiddenVSUnemploymentRate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="1080" windowWidth="24480" windowHeight="13400" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="25600" windowHeight="15740" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Shift-4M" sheetId="2" r:id="rId1"/>
@@ -105,8 +105,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -142,7 +148,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="37">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -158,6 +164,9 @@
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -173,6 +182,9 @@
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1280,11 +1292,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2098619992"/>
-        <c:axId val="-2104131160"/>
+        <c:axId val="-2087946328"/>
+        <c:axId val="-2087943288"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-2098619992"/>
+        <c:axId val="-2087946328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1294,14 +1306,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2104131160"/>
+        <c:crossAx val="-2087943288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-2104131160"/>
+        <c:axId val="-2087943288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1312,7 +1324,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2098619992"/>
+        <c:crossAx val="-2087946328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2441,11 +2453,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2097791688"/>
-        <c:axId val="-2116613368"/>
+        <c:axId val="2128748472"/>
+        <c:axId val="2129336136"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-2097791688"/>
+        <c:axId val="2128748472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2455,14 +2467,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2116613368"/>
+        <c:crossAx val="2129336136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-2116613368"/>
+        <c:axId val="2129336136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2473,14 +2485,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2097791688"/>
+        <c:crossAx val="2128748472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2593,11 +2604,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2113860440"/>
-        <c:axId val="-2098295224"/>
+        <c:axId val="-2087963192"/>
+        <c:axId val="-2087915704"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2113860440"/>
+        <c:axId val="-2087963192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2606,7 +2617,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2098295224"/>
+        <c:crossAx val="-2087915704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2614,7 +2625,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2098295224"/>
+        <c:axId val="-2087915704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2625,14 +2636,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2113860440"/>
+        <c:crossAx val="-2087963192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3507,11 +3517,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2123284072"/>
-        <c:axId val="-2095383448"/>
+        <c:axId val="-2113142392"/>
+        <c:axId val="-2117481752"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-2123284072"/>
+        <c:axId val="-2113142392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3521,14 +3531,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095383448"/>
+        <c:crossAx val="-2117481752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-2095383448"/>
+        <c:axId val="-2117481752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3539,14 +3549,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2123284072"/>
+        <c:crossAx val="-2113142392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4407,11 +4416,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2098675096"/>
-        <c:axId val="-2116106792"/>
+        <c:axId val="-2126238696"/>
+        <c:axId val="-2126248152"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-2098675096"/>
+        <c:axId val="-2126238696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4421,14 +4430,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2116106792"/>
+        <c:crossAx val="-2126248152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-2116106792"/>
+        <c:axId val="-2126248152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4439,7 +4448,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2098675096"/>
+        <c:crossAx val="-2126238696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4559,11 +4568,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2102453080"/>
-        <c:axId val="-2100104456"/>
+        <c:axId val="-2117580008"/>
+        <c:axId val="-2117289176"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2102453080"/>
+        <c:axId val="-2117580008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4572,7 +4581,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2100104456"/>
+        <c:crossAx val="-2117289176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4580,7 +4589,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2100104456"/>
+        <c:axId val="-2117289176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4591,7 +4600,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2102453080"/>
+        <c:crossAx val="-2117580008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4650,7 +4659,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="103" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="137" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
@@ -4777,7 +4786,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9210583" cy="5622524"/>
+    <xdr:ext cx="9214453" cy="5626934"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -6432,13 +6441,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="10" max="10" width="12.33203125" customWidth="1"/>
+    <col min="7" max="7" width="17.5" customWidth="1"/>
+    <col min="8" max="8" width="18" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" customWidth="1"/>
+    <col min="10" max="10" width="21.33203125" customWidth="1"/>
+    <col min="11" max="11" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">

</xml_diff>